<commit_message>
Changes as of 22-10-2023 in all classes(comments removed)
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/LoginData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1f42e9120523549/Desktop/Selenium files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony joseph\git\repository3\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC1048B7819F680A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AC878FE-B50B-41D3-B81D-54DD257CAAE4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB68BA5-F7C3-4E16-8FEA-941F5DFEC4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Emma</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -427,14 +430,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>

</xml_diff>